<commit_message>
Foi adicionado a função para pegar as informãções do jogo e armazenar em um arquivo excel
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -1,38 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,18 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -130,7 +211,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -165,7 +245,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -341,13 +420,354 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Multiplicador</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Pontos</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Batalhas</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ValorApostado</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ValorAcumulado</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Resultado</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-240</v>
+      </c>
+      <c r="D2" t="n">
+        <v>45</v>
+      </c>
+      <c r="E2" t="n">
+        <v>40.43</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>57</v>
+      </c>
+      <c r="D3" t="n">
+        <v>219</v>
+      </c>
+      <c r="E3" t="n">
+        <v>41.01</v>
+      </c>
+      <c r="F3" t="n">
+        <v>82.02</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1210</v>
+      </c>
+      <c r="D4" t="n">
+        <v>121</v>
+      </c>
+      <c r="E4" t="n">
+        <v>34.32</v>
+      </c>
+      <c r="F4" t="n">
+        <v>68.64</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>60</v>
+      </c>
+      <c r="E5" t="n">
+        <v>34.32</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>17</v>
+      </c>
+      <c r="E6" t="n">
+        <v>13.43</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1210</v>
+      </c>
+      <c r="D7" t="n">
+        <v>131</v>
+      </c>
+      <c r="E7" t="n">
+        <v>23.32</v>
+      </c>
+      <c r="F7" t="n">
+        <v>46.64</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>11</v>
+      </c>
+      <c r="E8" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1010</v>
+      </c>
+      <c r="D9" t="n">
+        <v>101</v>
+      </c>
+      <c r="E9" t="n">
+        <v>99.31999999999999</v>
+      </c>
+      <c r="F9" t="n">
+        <v>198.64</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>99.23</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.9846</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Nenhum</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-114</v>
+      </c>
+      <c r="D11" t="n">
+        <v>21</v>
+      </c>
+      <c r="E11" t="n">
+        <v>55.33</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="n">
+        <v>670</v>
+      </c>
+      <c r="D12" t="n">
+        <v>117</v>
+      </c>
+      <c r="E12" t="n">
+        <v>23.32</v>
+      </c>
+      <c r="F12" t="n">
+        <v>46.64</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Foi inserido uma descrição para o usuário apertar Enter após finalizar o jogo, isso vai fazer ativar o break
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,6 +767,222 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>960</v>
+      </c>
+      <c r="D13" t="n">
+        <v>106</v>
+      </c>
+      <c r="E13" t="n">
+        <v>23.32</v>
+      </c>
+      <c r="F13" t="n">
+        <v>46.64</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>379</v>
+      </c>
+      <c r="D14" t="n">
+        <v>225</v>
+      </c>
+      <c r="E14" t="n">
+        <v>20</v>
+      </c>
+      <c r="F14" t="n">
+        <v>40</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2.369999999999992</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>396</v>
+      </c>
+      <c r="E15" t="n">
+        <v>20</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2.369999999999992</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>397</v>
+      </c>
+      <c r="E16" t="n">
+        <v>20</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>746</v>
+      </c>
+      <c r="D17" t="n">
+        <v>172</v>
+      </c>
+      <c r="E17" t="n">
+        <v>40</v>
+      </c>
+      <c r="F17" t="n">
+        <v>80</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1030</v>
+      </c>
+      <c r="D18" t="n">
+        <v>113</v>
+      </c>
+      <c r="E18" t="n">
+        <v>100</v>
+      </c>
+      <c r="F18" t="n">
+        <v>200</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-170</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" t="n">
+        <v>30</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1047</v>
+      </c>
+      <c r="D20" t="n">
+        <v>120</v>
+      </c>
+      <c r="E20" t="n">
+        <v>20</v>
+      </c>
+      <c r="F20" t="n">
+        <v>40</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
O item de aumento de poder foi nerfado em quantidade de poder de 1000 a 5000 para 500 a 2500, teve o aumento da quantidade de 2 para 4, a chance de aparecer aumentou de 1 em 20 para 1 em 30. O tempo de espera ao encontrar o boss infernal diminiui de 3s para 2s
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1064,6 +1064,114 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" t="n">
+        <v>660</v>
+      </c>
+      <c r="D24" t="n">
+        <v>136</v>
+      </c>
+      <c r="E24" t="n">
+        <v>100</v>
+      </c>
+      <c r="F24" t="n">
+        <v>200</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1128</v>
+      </c>
+      <c r="D25" t="n">
+        <v>127</v>
+      </c>
+      <c r="E25" t="n">
+        <v>100</v>
+      </c>
+      <c r="F25" t="n">
+        <v>200</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2.099999999999998</v>
+      </c>
+      <c r="C26" t="n">
+        <v>828</v>
+      </c>
+      <c r="D26" t="n">
+        <v>137</v>
+      </c>
+      <c r="E26" t="n">
+        <v>100</v>
+      </c>
+      <c r="F26" t="n">
+        <v>209.9999999999998</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="n">
+        <v>980</v>
+      </c>
+      <c r="D27" t="n">
+        <v>146</v>
+      </c>
+      <c r="E27" t="n">
+        <v>40</v>
+      </c>
+      <c r="F27" t="n">
+        <v>80</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Foi ajustado o erro onde quando o boss infernal deixava o usuário com o poder => 0 ele ficava negativo. O item de aumento de poder teve a chance de aparecimento reduzida de 1 em 30 para 1 a 50
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1172,6 +1172,195 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>11</v>
+      </c>
+      <c r="E28" t="n">
+        <v>40</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" t="n">
+        <v>720</v>
+      </c>
+      <c r="D29" t="n">
+        <v>130</v>
+      </c>
+      <c r="E29" t="n">
+        <v>50</v>
+      </c>
+      <c r="F29" t="n">
+        <v>100</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>56</v>
+      </c>
+      <c r="E30" t="n">
+        <v>40</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.7600000000000005</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-619</v>
+      </c>
+      <c r="D31" t="n">
+        <v>208</v>
+      </c>
+      <c r="E31" t="n">
+        <v>20</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C32" t="n">
+        <v>10</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>200</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1070</v>
+      </c>
+      <c r="D33" t="n">
+        <v>107</v>
+      </c>
+      <c r="E33" t="n">
+        <v>20</v>
+      </c>
+      <c r="F33" t="n">
+        <v>40</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1070</v>
+      </c>
+      <c r="D34" t="n">
+        <v>124</v>
+      </c>
+      <c r="E34" t="n">
+        <v>21</v>
+      </c>
+      <c r="F34" t="n">
+        <v>42</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Foi ajustado o problema quando o usuário perdia e havia alguma pontuação, o sistema gerava um valor como recompensa
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1361,6 +1361,33 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C35" t="n">
+        <v>10</v>
+      </c>
+      <c r="D35" t="n">
+        <v>6</v>
+      </c>
+      <c r="E35" t="n">
+        <v>100</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Apareceu um problema ao remover a condicional de poder minimo para considerar a partida encerrada, foi reajustado para o default
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1388,6 +1388,87 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>7</v>
+      </c>
+      <c r="E36" t="n">
+        <v>100</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" t="n">
+        <v>810</v>
+      </c>
+      <c r="D37" t="n">
+        <v>111</v>
+      </c>
+      <c r="E37" t="n">
+        <v>13</v>
+      </c>
+      <c r="F37" t="n">
+        <v>26</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" t="n">
+        <v>920</v>
+      </c>
+      <c r="D38" t="n">
+        <v>137</v>
+      </c>
+      <c r="E38" t="n">
+        <v>70</v>
+      </c>
+      <c r="F38" t="n">
+        <v>140</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Alteração na informação onde o usuário encontra o Boss infernal, foi ajustado a palavra 'ULTMATE' para 'ULTIMATE'
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1496,6 +1496,87 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>68</v>
+      </c>
+      <c r="E40" t="n">
+        <v>40.3</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>11</v>
+      </c>
+      <c r="E41" t="n">
+        <v>20</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" t="n">
+        <v>10</v>
+      </c>
+      <c r="D42" t="n">
+        <v>207</v>
+      </c>
+      <c r="E42" t="n">
+        <v>40</v>
+      </c>
+      <c r="F42" t="n">
+        <v>80</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Foi feito uma classe para inserir os itens do jogo, os trechos de código repetidos contendo os itens atuais foram excluídos."
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1577,6 +1577,195 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>49</v>
+      </c>
+      <c r="E43" t="n">
+        <v>100</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>25</v>
+      </c>
+      <c r="E44" t="n">
+        <v>20</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>22</v>
+      </c>
+      <c r="E45" t="n">
+        <v>200</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-40</v>
+      </c>
+      <c r="D46" t="n">
+        <v>156</v>
+      </c>
+      <c r="E46" t="n">
+        <v>100</v>
+      </c>
+      <c r="F46" t="n">
+        <v>200</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>21</v>
+      </c>
+      <c r="E47" t="n">
+        <v>20</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" t="n">
+        <v>500</v>
+      </c>
+      <c r="D48" t="n">
+        <v>132</v>
+      </c>
+      <c r="E48" t="n">
+        <v>20</v>
+      </c>
+      <c r="F48" t="n">
+        <v>40</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" t="n">
+        <v>810</v>
+      </c>
+      <c r="D49" t="n">
+        <v>131</v>
+      </c>
+      <c r="E49" t="n">
+        <v>100</v>
+      </c>
+      <c r="F49" t="n">
+        <v>200</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
As funções dos itens agora recebem parâmetros ao invés de fazer uso de variáveis globais. Foi feito um ajuste na pontuação, todo começo de partida caso a pontuação seja menor que zero, o sistema deixará a pontuação em zero
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,6 +1766,114 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" t="n">
+        <v>960</v>
+      </c>
+      <c r="D50" t="n">
+        <v>96</v>
+      </c>
+      <c r="E50" t="n">
+        <v>100</v>
+      </c>
+      <c r="F50" t="n">
+        <v>200</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>17</v>
+      </c>
+      <c r="E51" t="n">
+        <v>100</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" t="n">
+        <v>760</v>
+      </c>
+      <c r="D52" t="n">
+        <v>96</v>
+      </c>
+      <c r="E52" t="n">
+        <v>100</v>
+      </c>
+      <c r="F52" t="n">
+        <v>200</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" t="n">
+        <v>980</v>
+      </c>
+      <c r="D53" t="n">
+        <v>98</v>
+      </c>
+      <c r="E53" t="n">
+        <v>100</v>
+      </c>
+      <c r="F53" t="n">
+        <v>200</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
A função de rugido foi colocada dentro do arquivo de funções. Foi criado uma pasta para testar as funções.
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -1,68 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ExerciciosGit\ScriptsExecutaveis\JogoDoPoder_v1.0\app\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Multiplicador</t>
-  </si>
-  <si>
-    <t>Pontos</t>
-  </si>
-  <si>
-    <t>Batalhas</t>
-  </si>
-  <si>
-    <t>ValorApostado</t>
-  </si>
-  <si>
-    <t>ValorAcumulado</t>
-  </si>
-  <si>
-    <t>Resultado</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -77,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -401,36 +420,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Multiplicador</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Pontos</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Batalhas</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ValorApostado</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ValorAcumulado</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Resultado</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+      <c r="C2" t="n">
+        <v>980</v>
+      </c>
+      <c r="D2" t="n">
+        <v>102</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="n">
+        <v>200</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>780</v>
+      </c>
+      <c r="D3" t="n">
+        <v>98</v>
+      </c>
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="n">
+        <v>200</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug onde o item de skipBoss não era consumido resolvido, a função de aumento de poder foi retirada da classe de Itens
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,222 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>680</v>
+      </c>
+      <c r="D4" t="n">
+        <v>105</v>
+      </c>
+      <c r="E4" t="n">
+        <v>100</v>
+      </c>
+      <c r="F4" t="n">
+        <v>200</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>760</v>
+      </c>
+      <c r="D5" t="n">
+        <v>96</v>
+      </c>
+      <c r="E5" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" t="n">
+        <v>200</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>960</v>
+      </c>
+      <c r="D6" t="n">
+        <v>96</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" t="n">
+        <v>40</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>11</v>
+      </c>
+      <c r="E7" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>990</v>
+      </c>
+      <c r="D8" t="n">
+        <v>99</v>
+      </c>
+      <c r="E8" t="n">
+        <v>100</v>
+      </c>
+      <c r="F8" t="n">
+        <v>200</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>990</v>
+      </c>
+      <c r="D9" t="n">
+        <v>99</v>
+      </c>
+      <c r="E9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F9" t="n">
+        <v>200</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>11</v>
+      </c>
+      <c r="E10" t="n">
+        <v>100</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="n">
+        <v>960</v>
+      </c>
+      <c r="D11" t="n">
+        <v>96</v>
+      </c>
+      <c r="E11" t="n">
+        <v>20</v>
+      </c>
+      <c r="F11" t="n">
+        <v>40</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
A função do item choiceBonus foi incluida na classe de Itens
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,6 +740,141 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>22</v>
+      </c>
+      <c r="E12" t="n">
+        <v>100</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>23</v>
+      </c>
+      <c r="E13" t="n">
+        <v>100</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>980</v>
+      </c>
+      <c r="D14" t="n">
+        <v>98</v>
+      </c>
+      <c r="E14" t="n">
+        <v>100</v>
+      </c>
+      <c r="F14" t="n">
+        <v>200</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="n">
+        <v>560</v>
+      </c>
+      <c r="D15" t="n">
+        <v>96</v>
+      </c>
+      <c r="E15" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" t="n">
+        <v>200</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>960</v>
+      </c>
+      <c r="D16" t="n">
+        <v>96</v>
+      </c>
+      <c r="E16" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" t="n">
+        <v>200</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Chance de pegar o bonus de poder aumentado de 1 em 50 para 1 em 45. Os monstros foram buffados em questão de poder inicial em +100.
</commit_message>
<xml_diff>
--- a/app/data/storage.xlsx
+++ b/app/data/storage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -875,6 +875,168 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>760</v>
+      </c>
+      <c r="D17" t="n">
+        <v>96</v>
+      </c>
+      <c r="E17" t="n">
+        <v>100</v>
+      </c>
+      <c r="F17" t="n">
+        <v>200</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" t="n">
+        <v>770</v>
+      </c>
+      <c r="D18" t="n">
+        <v>97</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
+        <v>20</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" t="n">
+        <v>570</v>
+      </c>
+      <c r="D19" t="n">
+        <v>98</v>
+      </c>
+      <c r="E19" t="n">
+        <v>100</v>
+      </c>
+      <c r="F19" t="n">
+        <v>200</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SkipBoss</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" t="n">
+        <v>759</v>
+      </c>
+      <c r="D20" t="n">
+        <v>104</v>
+      </c>
+      <c r="E20" t="n">
+        <v>20</v>
+      </c>
+      <c r="F20" t="n">
+        <v>40</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>14</v>
+      </c>
+      <c r="E21" t="n">
+        <v>100</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BonusPower</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" t="n">
+        <v>780</v>
+      </c>
+      <c r="D22" t="n">
+        <v>98</v>
+      </c>
+      <c r="E22" t="n">
+        <v>100</v>
+      </c>
+      <c r="F22" t="n">
+        <v>200</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>